<commit_message>
some random error forced me to commit again
some random error forced me to commit again
</commit_message>
<xml_diff>
--- a/Factors and Ridership Data/Model Estimation/Est7/FAC  7-4.xlsx
+++ b/Factors and Ridership Data/Model Estimation/Est7/FAC  7-4.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UoK\OneDrive - University of Kentucky\github\Transit_ridership\transit_ridership_decline\Factors and Ridership Data\Model Estimation\Est7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_3ED10CAE8D821312B89480C85AE1F592607CD07F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0928FDC7-5C98-48AC-A3A8-62641A313375}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_3ED10CAE8D821312B89480C85AE1F592607CD07F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CDB57A36-3040-4142-A883-B444C3B5D404}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="75" windowWidth="13380" windowHeight="15630" tabRatio="818" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="75" windowWidth="15045" windowHeight="15630" tabRatio="810" firstSheet="3" activeTab="6" xr2:uid="{1BE5E6F0-6B73-4BB7-902A-09A26060008F}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary-Bus" sheetId="21" r:id="rId1"/>
@@ -502,7 +503,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -838,6 +839,133 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1160,6 +1288,7 @@
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1651,7 +1780,7 @@
       </c>
       <c r="G10" s="67">
         <f>'FAC 2002-2018 BUS'!AD18</f>
-        <v>2.5416549662087624E-2</v>
+        <v>4.5418141738841032E-2</v>
       </c>
       <c r="H10" s="67">
         <f>'FAC 2002-2018 BUS'!AD47</f>
@@ -1723,7 +1852,7 @@
       </c>
       <c r="G11" s="67">
         <f>'FAC 2002-2018 BUS'!AD19</f>
-        <v>-5.1571731946016917E-3</v>
+        <v>-7.1051687933072127E-3</v>
       </c>
       <c r="H11" s="67">
         <f>'FAC 2002-2018 BUS'!AD48</f>
@@ -2330,9 +2459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:U24"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3571,9 +3699,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AG119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3588,11 +3717,16 @@
     <col min="10" max="10" width="11" style="15" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="24.625" style="15" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="12.625" style="15" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="13.625" style="15" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.125" style="15" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="11.125" style="15" hidden="1" customWidth="1"/>
-    <col min="16" max="28" width="11.625" style="15" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="10" style="15" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="11" style="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="10.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="24" max="28" width="10.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10" style="15" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12.125" style="15" customWidth="1"/>
     <col min="31" max="31" width="17.5" style="13" bestFit="1" customWidth="1"/>
     <col min="32" max="16384" width="11" style="15"/>
@@ -3871,7 +4005,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:31" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="28"/>
       <c r="C10" s="31"/>
@@ -3936,237 +4070,237 @@
       <c r="AD10" s="9"/>
       <c r="AE10" s="9"/>
     </row>
-    <row r="11" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="str">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B11" s="124"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="111" t="str">
         <f>CONCATENATE($C6,"_",$C7,"_",G9)</f>
         <v>0_1_2002</v>
       </c>
-      <c r="H11" s="9" t="str">
+      <c r="H11" s="111" t="str">
         <f>CONCATENATE($C6,"_",$C7,"_",H9)</f>
         <v>0_1_2018</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9" t="str">
+      <c r="I11" s="125"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="111"/>
+      <c r="L11" s="111"/>
+      <c r="M11" s="111" t="str">
         <f>IF($G9+M10&gt;$H9,0,CONCATENATE($C6,"_",$C7,"_",$G9+M10))</f>
         <v>0_1_2003</v>
       </c>
-      <c r="N11" s="9" t="str">
+      <c r="N11" s="111" t="str">
         <f t="shared" ref="N11:AB11" si="0">IF($G9+N10&gt;$H9,0,CONCATENATE($C6,"_",$C7,"_",$G9+N10))</f>
         <v>0_1_2004</v>
       </c>
-      <c r="O11" s="9" t="str">
+      <c r="O11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2005</v>
       </c>
-      <c r="P11" s="9" t="str">
+      <c r="P11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2006</v>
       </c>
-      <c r="Q11" s="9" t="str">
+      <c r="Q11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2007</v>
       </c>
-      <c r="R11" s="9" t="str">
+      <c r="R11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2008</v>
       </c>
-      <c r="S11" s="9" t="str">
+      <c r="S11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2009</v>
       </c>
-      <c r="T11" s="9" t="str">
+      <c r="T11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2010</v>
       </c>
-      <c r="U11" s="9" t="str">
+      <c r="U11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2011</v>
       </c>
-      <c r="V11" s="9" t="str">
+      <c r="V11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2012</v>
       </c>
-      <c r="W11" s="9" t="str">
+      <c r="W11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2013</v>
       </c>
-      <c r="X11" s="9" t="str">
+      <c r="X11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2014</v>
       </c>
-      <c r="Y11" s="9" t="str">
+      <c r="Y11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2015</v>
       </c>
-      <c r="Z11" s="9" t="str">
+      <c r="Z11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2016</v>
       </c>
-      <c r="AA11" s="9" t="str">
+      <c r="AA11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2017</v>
       </c>
-      <c r="AB11" s="9" t="str">
+      <c r="AB11" s="111" t="str">
         <f t="shared" si="0"/>
         <v>0_1_2018</v>
       </c>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-    </row>
-    <row r="12" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9" t="s">
+      <c r="AC11" s="111"/>
+      <c r="AD11" s="111"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B12" s="124"/>
+      <c r="C12" s="125"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9" t="s">
+      <c r="G12" s="126"/>
+      <c r="H12" s="126"/>
+      <c r="I12" s="125"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="111"/>
+      <c r="L12" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
+      <c r="M12" s="111"/>
+      <c r="N12" s="111"/>
+      <c r="O12" s="111"/>
+      <c r="P12" s="111"/>
+      <c r="Q12" s="111"/>
+      <c r="R12" s="111"/>
+      <c r="S12" s="111"/>
+      <c r="T12" s="111"/>
+      <c r="U12" s="111"/>
+      <c r="V12" s="111"/>
+      <c r="W12" s="111"/>
+      <c r="X12" s="111"/>
+      <c r="Y12" s="111"/>
+      <c r="Z12" s="111"/>
+      <c r="AA12" s="111"/>
+      <c r="AB12" s="111"/>
+      <c r="AC12" s="111"/>
+      <c r="AD12" s="111"/>
     </row>
     <row r="13" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="59">
+      <c r="E13" s="127">
         <v>0.83279999999999998</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="111">
         <f>MATCH($D13,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>11</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="126">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F13,FALSE)</f>
         <v>50210669.002108097</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="126">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F13,FALSE)</f>
         <v>51942398.1681339</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="128">
         <f>IFERROR(H13/G13-1,"-")</f>
         <v>3.4489266931557738E-2</v>
       </c>
-      <c r="J13" s="34" t="str">
+      <c r="J13" s="129" t="str">
         <f>IF(C13="Log","_log","")</f>
         <v>_log</v>
       </c>
-      <c r="K13" s="34" t="str">
+      <c r="K13" s="129" t="str">
         <f>CONCATENATE(D13,J13,"_FAC")</f>
         <v>VRM_ADJ_log_FAC</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="111">
         <f>MATCH($K13,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>25</v>
       </c>
-      <c r="M13" s="32">
+      <c r="M13" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>73668137.884693295</v>
       </c>
-      <c r="N13" s="32">
+      <c r="N13" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>14858985.975418899</v>
       </c>
-      <c r="O13" s="32">
+      <c r="O13" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>-34748716.953290999</v>
       </c>
-      <c r="P13" s="32">
+      <c r="P13" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>5598070.7876798697</v>
       </c>
-      <c r="Q13" s="32">
+      <c r="Q13" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>39707341.847191297</v>
       </c>
-      <c r="R13" s="32">
+      <c r="R13" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>35569324.878848098</v>
       </c>
-      <c r="S13" s="32">
+      <c r="S13" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>-4782853.4183069998</v>
       </c>
-      <c r="T13" s="32">
+      <c r="T13" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>-71064888.041222095</v>
       </c>
-      <c r="U13" s="32">
+      <c r="U13" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>-40181533.355351098</v>
       </c>
-      <c r="V13" s="32">
+      <c r="V13" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>-13607589.765833801</v>
       </c>
-      <c r="W13" s="32">
+      <c r="W13" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>30261105.473729301</v>
       </c>
-      <c r="X13" s="32">
+      <c r="X13" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>6998942.5925363703</v>
       </c>
-      <c r="Y13" s="32">
+      <c r="Y13" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>32676381.4395556</v>
       </c>
-      <c r="Z13" s="32">
+      <c r="Z13" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>21557904.3169882</v>
       </c>
-      <c r="AA13" s="32">
+      <c r="AA13" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>17103963.4136011</v>
       </c>
-      <c r="AB13" s="32">
+      <c r="AB13" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L13,FALSE))</f>
         <v>10304113.396397701</v>
       </c>
-      <c r="AC13" s="35">
+      <c r="AC13" s="130">
         <f>SUM(M13:AB13)</f>
         <v>123918690.47263472</v>
       </c>
-      <c r="AD13" s="36">
+      <c r="AD13" s="131">
         <f>AC13/G29</f>
         <v>6.2521860796382653E-2</v>
       </c>
@@ -4174,115 +4308,115 @@
     </row>
     <row r="14" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="124" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="59">
+      <c r="E14" s="127">
         <v>-0.59099999999999997</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="111">
         <f>MATCH($D14,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>12</v>
       </c>
-      <c r="G14" s="58">
+      <c r="G14" s="132">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F14,FALSE)</f>
         <v>0.96214307337159199</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="132">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F14,FALSE)</f>
         <v>1.0767597388407599</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I14" s="128">
         <f t="shared" ref="I14:I26" si="1">IFERROR(H14/G14-1,"-")</f>
         <v>0.11912642583137067</v>
       </c>
-      <c r="J14" s="34" t="str">
+      <c r="J14" s="129" t="str">
         <f t="shared" ref="J14:J26" si="2">IF(C14="Log","_log","")</f>
         <v>_log</v>
       </c>
-      <c r="K14" s="34" t="str">
+      <c r="K14" s="129" t="str">
         <f t="shared" ref="K14:K27" si="3">CONCATENATE(D14,J14,"_FAC")</f>
         <v>FARE_per_UPT_2018_log_FAC</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="111">
         <f>MATCH($K14,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>26</v>
       </c>
-      <c r="M14" s="32">
+      <c r="M14" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>23451013.618424099</v>
       </c>
-      <c r="N14" s="32">
+      <c r="N14" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>-15039078.3063318</v>
       </c>
-      <c r="O14" s="32">
+      <c r="O14" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>-5217099.7383297104</v>
       </c>
-      <c r="P14" s="32">
+      <c r="P14" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>10082024.061600599</v>
       </c>
-      <c r="Q14" s="32">
+      <c r="Q14" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>-20385941.4434014</v>
       </c>
-      <c r="R14" s="32">
+      <c r="R14" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>25255273.607143201</v>
       </c>
-      <c r="S14" s="32">
+      <c r="S14" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>-63621596.392088503</v>
       </c>
-      <c r="T14" s="32">
+      <c r="T14" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>-17824527.549885601</v>
       </c>
-      <c r="U14" s="32">
+      <c r="U14" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>15322710.399470299</v>
       </c>
-      <c r="V14" s="32">
+      <c r="V14" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>-22340810.702362701</v>
       </c>
-      <c r="W14" s="32">
+      <c r="W14" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>-16125712.701229</v>
       </c>
-      <c r="X14" s="32">
+      <c r="X14" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>-129556.862135185</v>
       </c>
-      <c r="Y14" s="32">
+      <c r="Y14" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>-9885858.7926116195</v>
       </c>
-      <c r="Z14" s="32">
+      <c r="Z14" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>-10670628.621276701</v>
       </c>
-      <c r="AA14" s="32">
+      <c r="AA14" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>18645283.2225587</v>
       </c>
-      <c r="AB14" s="32">
+      <c r="AB14" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L14,FALSE))</f>
         <v>15350149.852120001</v>
       </c>
-      <c r="AC14" s="35">
+      <c r="AC14" s="130">
         <f t="shared" ref="AC14:AC26" si="4">SUM(M14:AB14)</f>
         <v>-73134356.348335341</v>
       </c>
-      <c r="AD14" s="36">
+      <c r="AD14" s="131">
         <f>AC14/G29</f>
         <v>-3.689916371456025E-2</v>
       </c>
@@ -4290,115 +4424,115 @@
     </row>
     <row r="15" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="59">
+      <c r="E15" s="127">
         <v>0.37669999999999998</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="111">
         <f>MATCH($D15,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>13</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="126">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F15,FALSE)</f>
         <v>6960297.26032863</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="126">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F15,FALSE)</f>
         <v>8481156.0926418807</v>
       </c>
-      <c r="I15" s="33">
+      <c r="I15" s="128">
         <f t="shared" si="1"/>
         <v>0.21850486774201983</v>
       </c>
-      <c r="J15" s="34" t="str">
+      <c r="J15" s="129" t="str">
         <f t="shared" si="2"/>
         <v>_log</v>
       </c>
-      <c r="K15" s="34" t="str">
+      <c r="K15" s="129" t="str">
         <f t="shared" si="3"/>
         <v>POP_EMP_log_FAC</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="111">
         <f>MATCH($K15,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>27</v>
       </c>
-      <c r="M15" s="32">
+      <c r="M15" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>14890801.861083699</v>
       </c>
-      <c r="N15" s="32">
+      <c r="N15" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>17960858.0823141</v>
       </c>
-      <c r="O15" s="32">
+      <c r="O15" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>18346612.535783499</v>
       </c>
-      <c r="P15" s="32">
+      <c r="P15" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>23350125.553405002</v>
       </c>
-      <c r="Q15" s="32">
+      <c r="Q15" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>7751177.7756346799</v>
       </c>
-      <c r="R15" s="32">
+      <c r="R15" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>5683929.5188827598</v>
       </c>
-      <c r="S15" s="32">
+      <c r="S15" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>-1473131.0837824</v>
       </c>
-      <c r="T15" s="32">
+      <c r="T15" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>2002182.0492676401</v>
       </c>
-      <c r="U15" s="32">
+      <c r="U15" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>8497432.3227526695</v>
       </c>
-      <c r="V15" s="32">
+      <c r="V15" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>10577677.354012599</v>
       </c>
-      <c r="W15" s="32">
+      <c r="W15" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>9645146.6889573894</v>
       </c>
-      <c r="X15" s="32">
+      <c r="X15" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>11289444.2067378</v>
       </c>
-      <c r="Y15" s="32">
+      <c r="Y15" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>10214784.090726599</v>
       </c>
-      <c r="Z15" s="32">
+      <c r="Z15" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>8134768.24412861</v>
       </c>
-      <c r="AA15" s="32">
+      <c r="AA15" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>9267335.8062921297</v>
       </c>
-      <c r="AB15" s="32">
+      <c r="AB15" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L15,FALSE))</f>
         <v>7689236.0380116804</v>
       </c>
-      <c r="AC15" s="35">
+      <c r="AC15" s="130">
         <f t="shared" si="4"/>
         <v>163828381.04420844</v>
       </c>
-      <c r="AD15" s="36">
+      <c r="AD15" s="131">
         <f>AC15/G29</f>
         <v>8.265787182769406E-2</v>
       </c>
@@ -4406,113 +4540,113 @@
     </row>
     <row r="16" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="124" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="9" t="s">
+      <c r="C16" s="125"/>
+      <c r="D16" s="111" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="59">
+      <c r="E16" s="127">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="111">
         <f>MATCH($D16,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>17</v>
       </c>
-      <c r="G16" s="58">
+      <c r="G16" s="132">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F16,FALSE)</f>
         <v>51.770454283682596</v>
       </c>
-      <c r="H16" s="58">
+      <c r="H16" s="132">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F16,FALSE)</f>
         <v>41.073403477542698</v>
       </c>
-      <c r="I16" s="33">
+      <c r="I16" s="128">
         <f t="shared" si="1"/>
         <v>-0.20662462700296369</v>
       </c>
-      <c r="J16" s="34" t="str">
+      <c r="J16" s="129" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K16" s="34" t="str">
+      <c r="K16" s="129" t="str">
         <f t="shared" si="3"/>
         <v>TSD_POP_PCT_FAC</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="111">
         <f>MATCH($K16,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>31</v>
       </c>
-      <c r="M16" s="32">
+      <c r="M16" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>-20824628.856763002</v>
       </c>
-      <c r="N16" s="32">
+      <c r="N16" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>-19744158.019365001</v>
       </c>
-      <c r="O16" s="32">
+      <c r="O16" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>-17712133.750411</v>
       </c>
-      <c r="P16" s="32">
+      <c r="P16" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>-19862488.235452302</v>
       </c>
-      <c r="Q16" s="32">
+      <c r="Q16" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>-7098774.9855081597</v>
       </c>
-      <c r="R16" s="32">
+      <c r="R16" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>-8704013.40038619</v>
       </c>
-      <c r="S16" s="32">
+      <c r="S16" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>-11280334.2594142</v>
       </c>
-      <c r="T16" s="32">
+      <c r="T16" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>-5563187.4459224399</v>
       </c>
-      <c r="U16" s="32">
+      <c r="U16" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>-8375600.4785643797</v>
       </c>
-      <c r="V16" s="32">
+      <c r="V16" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>-343883.12016486999</v>
       </c>
-      <c r="W16" s="32">
+      <c r="W16" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>-295501.26651126298</v>
       </c>
-      <c r="X16" s="32">
+      <c r="X16" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>200984.945279023</v>
       </c>
-      <c r="Y16" s="32">
+      <c r="Y16" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>434922.44341572298</v>
       </c>
-      <c r="Z16" s="32">
+      <c r="Z16" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>1028974.8868583801</v>
       </c>
-      <c r="AA16" s="32">
+      <c r="AA16" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>374237.54468727298</v>
       </c>
-      <c r="AB16" s="32">
+      <c r="AB16" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L16,FALSE))</f>
         <v>501951.30948506598</v>
       </c>
-      <c r="AC16" s="35">
+      <c r="AC16" s="130">
         <f t="shared" si="4"/>
         <v>-117263632.68873736</v>
       </c>
-      <c r="AD16" s="36">
+      <c r="AD16" s="131">
         <f>AC16/G29</f>
         <v>-5.9164121985798637E-2</v>
       </c>
@@ -4520,115 +4654,115 @@
     </row>
     <row r="17" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="124" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="59">
+      <c r="E17" s="127">
         <v>0.1762</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="111">
         <f>MATCH($D17,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>14</v>
       </c>
-      <c r="G17" s="37">
+      <c r="G17" s="134">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F17,FALSE)</f>
         <v>1.9678602713629301</v>
       </c>
-      <c r="H17" s="37">
+      <c r="H17" s="134">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F17,FALSE)</f>
         <v>2.9560754566985299</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="128">
         <f t="shared" si="1"/>
         <v>0.50217751723356208</v>
       </c>
-      <c r="J17" s="34" t="str">
+      <c r="J17" s="129" t="str">
         <f t="shared" si="2"/>
         <v>_log</v>
       </c>
-      <c r="K17" s="34" t="str">
+      <c r="K17" s="129" t="str">
         <f t="shared" si="3"/>
         <v>GAS_PRICE_2018_log_FAC</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="111">
         <f>MATCH($K17,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>28</v>
       </c>
-      <c r="M17" s="32">
+      <c r="M17" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>32104661.904764201</v>
       </c>
-      <c r="N17" s="32">
+      <c r="N17" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>33217281.546094399</v>
       </c>
-      <c r="O17" s="32">
+      <c r="O17" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>43167395.657005802</v>
       </c>
-      <c r="P17" s="32">
+      <c r="P17" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>25074421.3214145</v>
       </c>
-      <c r="Q17" s="32">
+      <c r="Q17" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>13959297.741871299</v>
       </c>
-      <c r="R17" s="32">
+      <c r="R17" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>33276852.581209201</v>
       </c>
-      <c r="S17" s="32">
+      <c r="S17" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>-90147911.714342803</v>
       </c>
-      <c r="T17" s="32">
+      <c r="T17" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>41136548.147473998</v>
       </c>
-      <c r="U17" s="32">
+      <c r="U17" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>56740870.446837001</v>
       </c>
-      <c r="V17" s="32">
+      <c r="V17" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>2216451.6482136999</v>
       </c>
-      <c r="W17" s="32">
+      <c r="W17" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>-11868515.7724318</v>
       </c>
-      <c r="X17" s="32">
+      <c r="X17" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>-15741770.3392531</v>
       </c>
-      <c r="Y17" s="32">
+      <c r="Y17" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>-80372042.952035099</v>
       </c>
-      <c r="Z17" s="32">
+      <c r="Z17" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>-30757229.8204813</v>
       </c>
-      <c r="AA17" s="32">
+      <c r="AA17" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>21229304.2730776</v>
       </c>
-      <c r="AB17" s="32">
+      <c r="AB17" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L17,FALSE))</f>
         <v>24787534.827645499</v>
       </c>
-      <c r="AC17" s="35">
+      <c r="AC17" s="130">
         <f t="shared" si="4"/>
         <v>98023149.497063145</v>
       </c>
-      <c r="AD17" s="36">
+      <c r="AD17" s="131">
         <f>AC17/G29</f>
         <v>4.9456540287050405E-2</v>
       </c>
@@ -4636,343 +4770,343 @@
     </row>
     <row r="18" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="124" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="111" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="59">
+      <c r="E18" s="127">
         <v>-0.27529999999999999</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="111">
         <f>MATCH($D18,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>15</v>
       </c>
-      <c r="G18" s="58">
+      <c r="G18" s="132">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F18,FALSE)</f>
         <v>41470.960736725603</v>
       </c>
-      <c r="H18" s="58">
+      <c r="H18" s="132">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F18,FALSE)</f>
         <v>38094.696885668702</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="128">
         <f t="shared" si="1"/>
         <v>-8.1412723290660849E-2</v>
       </c>
-      <c r="J18" s="34" t="str">
+      <c r="J18" s="129" t="str">
         <f t="shared" si="2"/>
         <v>_log</v>
       </c>
-      <c r="K18" s="34" t="str">
+      <c r="K18" s="129" t="str">
         <f t="shared" si="3"/>
         <v>TOTAL_MED_INC_INDIV_2018_log_FAC</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="111">
         <f>MATCH($K18,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>29</v>
       </c>
-      <c r="M18" s="32">
+      <c r="M18" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>10466670.607873101</v>
       </c>
-      <c r="N18" s="32">
+      <c r="N18" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>15216253.2400127</v>
       </c>
-      <c r="O18" s="32">
+      <c r="O18" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>13908939.910751101</v>
       </c>
-      <c r="P18" s="32">
+      <c r="P18" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>22670853.326227099</v>
       </c>
-      <c r="Q18" s="32">
+      <c r="Q18" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>-8104038.1064764</v>
       </c>
-      <c r="R18" s="32">
+      <c r="R18" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>-675166.98916859599</v>
       </c>
-      <c r="S18" s="32">
+      <c r="S18" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>29211014.582727201</v>
       </c>
-      <c r="T18" s="32">
+      <c r="T18" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>15500007.4189585</v>
       </c>
-      <c r="U18" s="32">
+      <c r="U18" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
-        <v>8606390.5169233494</v>
-      </c>
-      <c r="V18" s="32">
+        <v>48249661.941476241</v>
+      </c>
+      <c r="V18" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>2904369.3381795702</v>
       </c>
-      <c r="W18" s="32">
+      <c r="W18" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>-4849996.3330890303</v>
       </c>
-      <c r="X18" s="32">
+      <c r="X18" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>-4929091.3576107798</v>
       </c>
-      <c r="Y18" s="32">
+      <c r="Y18" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>-18095714.298998799</v>
       </c>
-      <c r="Z18" s="32">
+      <c r="Z18" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>-11936511.7756317</v>
       </c>
-      <c r="AA18" s="32">
+      <c r="AA18" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>-9057946.9539233707</v>
       </c>
-      <c r="AB18" s="32">
+      <c r="AB18" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L18,FALSE))</f>
         <v>-10460284.383191099</v>
       </c>
-      <c r="AC18" s="35">
+      <c r="AC18" s="130">
         <f t="shared" si="4"/>
-        <v>50375748.743562855</v>
-      </c>
-      <c r="AD18" s="36">
+        <v>90019020.16811572</v>
+      </c>
+      <c r="AD18" s="131">
         <f>AC18/G29</f>
-        <v>2.5416549662087624E-2</v>
+        <v>4.5418141738841032E-2</v>
       </c>
       <c r="AE18" s="9"/>
     </row>
     <row r="19" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="124" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="9" t="s">
+      <c r="C19" s="125"/>
+      <c r="D19" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="59">
+      <c r="E19" s="127">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="111">
         <f>MATCH($D19,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>16</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="126">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F19,FALSE)</f>
         <v>10.2554362716791</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="126">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F19,FALSE)</f>
         <v>9.5234524029876901</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I19" s="128">
         <f t="shared" si="1"/>
         <v>-7.1375205237520722E-2</v>
       </c>
-      <c r="J19" s="34" t="str">
+      <c r="J19" s="129" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K19" s="34" t="str">
+      <c r="K19" s="129" t="str">
         <f t="shared" si="3"/>
         <v>PCT_HH_NO_VEH_FAC</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="111">
         <f>MATCH($K19,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>30</v>
       </c>
-      <c r="M19" s="32">
+      <c r="M19" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-1625621.61060477</v>
       </c>
-      <c r="N19" s="32">
+      <c r="N19" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-1671097.7800906899</v>
       </c>
-      <c r="O19" s="32">
+      <c r="O19" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-1885064.5419131301</v>
       </c>
-      <c r="P19" s="32">
+      <c r="P19" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-1525514.2877553899</v>
       </c>
-      <c r="Q19" s="32">
+      <c r="Q19" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-2592116.0127329198</v>
       </c>
-      <c r="R19" s="32">
+      <c r="R19" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>2466795.8584225602</v>
       </c>
-      <c r="S19" s="32">
+      <c r="S19" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>2238488.2148257201</v>
       </c>
-      <c r="T19" s="32">
+      <c r="T19" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>2916828.8596050399</v>
       </c>
-      <c r="U19" s="32">
+      <c r="U19" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
-        <v>3860938.6203019</v>
-      </c>
-      <c r="V19" s="32">
+        <v>5.3162988831291169E-2</v>
+      </c>
+      <c r="V19" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-1396245.7504827899</v>
       </c>
-      <c r="W19" s="32">
+      <c r="W19" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-3593957.3471187698</v>
       </c>
-      <c r="X19" s="32">
+      <c r="X19" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-637248.03456782398</v>
       </c>
-      <c r="Y19" s="32">
+      <c r="Y19" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-1061829.0654498399</v>
       </c>
-      <c r="Z19" s="32">
+      <c r="Z19" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-1693219.23886861</v>
       </c>
-      <c r="AA19" s="32">
+      <c r="AA19" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-2134344.2951190402</v>
       </c>
-      <c r="AB19" s="32">
+      <c r="AB19" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L19,FALSE))</f>
         <v>-1888340.75092155</v>
       </c>
-      <c r="AC19" s="35">
+      <c r="AC19" s="130">
         <f t="shared" si="4"/>
-        <v>-10221547.162470102</v>
-      </c>
-      <c r="AD19" s="36">
+        <v>-14082485.729609014</v>
+      </c>
+      <c r="AD19" s="131">
         <f>AC19/G29</f>
-        <v>-5.1571731946016917E-3</v>
+        <v>-7.1051687933072127E-3</v>
       </c>
       <c r="AE19" s="9"/>
     </row>
     <row r="20" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="124" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="9" t="s">
+      <c r="C20" s="125"/>
+      <c r="D20" s="111" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="59">
+      <c r="E20" s="127">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="111">
         <f>MATCH($D20,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>18</v>
       </c>
-      <c r="G20" s="37">
+      <c r="G20" s="134">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F20,FALSE)</f>
         <v>3.9479789383814201</v>
       </c>
-      <c r="H20" s="37">
+      <c r="H20" s="134">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F20,FALSE)</f>
         <v>6.1711602035772204</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="128">
         <f t="shared" si="1"/>
         <v>0.56311882608655783</v>
       </c>
-      <c r="J20" s="34" t="str">
+      <c r="J20" s="129" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K20" s="34" t="str">
+      <c r="K20" s="129" t="str">
         <f t="shared" si="3"/>
         <v>JTW_HOME_PCT_FAC</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="111">
         <f>MATCH($K20,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>32</v>
       </c>
-      <c r="M20" s="32">
+      <c r="M20" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="N20" s="32">
+      <c r="N20" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="O20" s="32">
+      <c r="O20" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="P20" s="32">
+      <c r="P20" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-2147363.8358005802</v>
       </c>
-      <c r="Q20" s="32">
+      <c r="Q20" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-731707.94856523594</v>
       </c>
-      <c r="R20" s="32">
+      <c r="R20" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-505423.53572935303</v>
       </c>
-      <c r="S20" s="32">
+      <c r="S20" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-1204891.4289271899</v>
       </c>
-      <c r="T20" s="32">
+      <c r="T20" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-1451770.7291632099</v>
       </c>
-      <c r="U20" s="32">
+      <c r="U20" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>414833.62961664802</v>
       </c>
-      <c r="V20" s="32">
+      <c r="V20" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-645260.62301078904</v>
       </c>
-      <c r="W20" s="32">
+      <c r="W20" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-7457.63808997043</v>
       </c>
-      <c r="X20" s="32">
+      <c r="X20" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-1256949.7416145999</v>
       </c>
-      <c r="Y20" s="32">
+      <c r="Y20" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-585177.17204295099</v>
       </c>
-      <c r="Z20" s="32">
+      <c r="Z20" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-3100839.9903968601</v>
       </c>
-      <c r="AA20" s="32">
+      <c r="AA20" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-948079.97853902902</v>
       </c>
-      <c r="AB20" s="32">
+      <c r="AB20" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L20,FALSE))</f>
         <v>-1401352.39163396</v>
       </c>
-      <c r="AC20" s="35">
+      <c r="AC20" s="130">
         <f t="shared" si="4"/>
         <v>-13571441.383897081</v>
       </c>
-      <c r="AD20" s="36">
+      <c r="AD20" s="131">
         <f>AC20/G29</f>
         <v>-6.8473267896392038E-3</v>
       </c>
@@ -4980,113 +5114,113 @@
     </row>
     <row r="21" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="14" t="s">
+      <c r="C21" s="125"/>
+      <c r="D21" s="135" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="59">
+      <c r="E21" s="127">
         <v>-1.29E-2</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="111">
         <f>MATCH($D21,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>19</v>
       </c>
-      <c r="G21" s="37">
+      <c r="G21" s="134">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F21,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="37">
+      <c r="H21" s="134">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F21,FALSE)</f>
         <v>7.2225746763552303</v>
       </c>
-      <c r="I21" s="33" t="str">
+      <c r="I21" s="128" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="J21" s="34" t="str">
+      <c r="J21" s="129" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K21" s="34" t="str">
+      <c r="K21" s="129" t="str">
         <f t="shared" si="3"/>
         <v>YEARS_SINCE_TNC_BUS2_HINY_FAC</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21" s="111">
         <f>MATCH($K21,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>33</v>
       </c>
-      <c r="M21" s="32">
+      <c r="M21" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="N21" s="32">
+      <c r="N21" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="O21" s="32">
+      <c r="O21" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="P21" s="32">
+      <c r="P21" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Q21" s="32">
+      <c r="Q21" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="R21" s="32">
+      <c r="R21" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="S21" s="32">
+      <c r="S21" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="T21" s="32">
+      <c r="T21" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>-3861484.5228403602</v>
       </c>
-      <c r="U21" s="32">
+      <c r="U21" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>-12057002.6989104</v>
       </c>
-      <c r="V21" s="32">
+      <c r="V21" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>-20082763.361682899</v>
       </c>
-      <c r="W21" s="32">
+      <c r="W21" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>-22492412.659255601</v>
       </c>
-      <c r="X21" s="32">
+      <c r="X21" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>-26645891.121726502</v>
       </c>
-      <c r="Y21" s="32">
+      <c r="Y21" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>-26507856.1955452</v>
       </c>
-      <c r="Z21" s="32">
+      <c r="Z21" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>-26086071.995433699</v>
       </c>
-      <c r="AA21" s="32">
+      <c r="AA21" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>-25005395.5115714</v>
       </c>
-      <c r="AB21" s="32">
+      <c r="AB21" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L21,FALSE))</f>
         <v>-24104353.595256999</v>
       </c>
-      <c r="AC21" s="35">
+      <c r="AC21" s="130">
         <f t="shared" si="4"/>
         <v>-186843231.66222304</v>
       </c>
-      <c r="AD21" s="36">
+      <c r="AD21" s="131">
         <f>AC21/G29</f>
         <v>-9.4269770574371137E-2</v>
       </c>
@@ -5094,113 +5228,113 @@
     </row>
     <row r="22" spans="1:31" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="14" t="s">
+      <c r="C22" s="125"/>
+      <c r="D22" s="135" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="59">
+      <c r="E22" s="127">
         <v>-2.7400000000000001E-2</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="111">
         <f>MATCH($D22,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>20</v>
       </c>
-      <c r="G22" s="37">
+      <c r="G22" s="134">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F22,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="37">
+      <c r="H22" s="134">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F22,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="33" t="str">
+      <c r="I22" s="128" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="J22" s="34" t="str">
+      <c r="J22" s="129" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K22" s="34" t="str">
+      <c r="K22" s="129" t="str">
         <f t="shared" si="3"/>
         <v>YEARS_SINCE_TNC_BUS2_MIDLOW_FAC</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L22" s="111">
         <f>MATCH($K22,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>34</v>
       </c>
-      <c r="M22" s="32">
+      <c r="M22" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="N22" s="32">
+      <c r="N22" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="O22" s="32">
+      <c r="O22" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="P22" s="32">
+      <c r="P22" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="32">
+      <c r="Q22" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="R22" s="32">
+      <c r="R22" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="S22" s="32">
+      <c r="S22" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="T22" s="32">
+      <c r="T22" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="U22" s="32">
+      <c r="U22" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="V22" s="32">
+      <c r="V22" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="W22" s="32">
+      <c r="W22" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="X22" s="32">
+      <c r="X22" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Y22" s="32">
+      <c r="Y22" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Z22" s="32">
+      <c r="Z22" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AA22" s="32">
+      <c r="AA22" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AB22" s="32">
+      <c r="AB22" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L22,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AC22" s="35">
+      <c r="AC22" s="130">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD22" s="36">
+      <c r="AD22" s="131">
         <f>AC22/G29</f>
         <v>0</v>
       </c>
@@ -5208,110 +5342,110 @@
     </row>
     <row r="23" spans="1:31" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="14" t="s">
+      <c r="C23" s="125"/>
+      <c r="D23" s="135" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="59">
+      <c r="E23" s="127">
         <v>-2.5999999999999999E-3</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="111">
         <f>MATCH($D23,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>21</v>
       </c>
-      <c r="G23" s="37">
+      <c r="G23" s="134">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F23,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H23" s="37">
+      <c r="H23" s="134">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F23,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I23" s="33" t="str">
+      <c r="I23" s="128" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34" t="str">
+      <c r="J23" s="129"/>
+      <c r="K23" s="129" t="str">
         <f t="shared" si="3"/>
         <v>YEARS_SINCE_TNC_RAIL2_HINY_FAC</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L23" s="111">
         <f>MATCH($K23,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>35</v>
       </c>
-      <c r="M23" s="32">
+      <c r="M23" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="N23" s="32">
+      <c r="N23" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="O23" s="32">
+      <c r="O23" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="P23" s="32">
+      <c r="P23" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="32">
+      <c r="Q23" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="R23" s="32">
+      <c r="R23" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="S23" s="32">
+      <c r="S23" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="T23" s="32">
+      <c r="T23" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="U23" s="32">
+      <c r="U23" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="V23" s="32">
+      <c r="V23" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="W23" s="32">
+      <c r="W23" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="X23" s="32">
+      <c r="X23" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Y23" s="32">
+      <c r="Y23" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Z23" s="32">
+      <c r="Z23" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AA23" s="32">
+      <c r="AA23" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AB23" s="32">
+      <c r="AB23" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L23,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AC23" s="35">
+      <c r="AC23" s="130">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD23" s="36">
+      <c r="AD23" s="131">
         <f>AC23/G29</f>
         <v>0</v>
       </c>
@@ -5319,110 +5453,110 @@
     </row>
     <row r="24" spans="1:31" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="14" t="s">
+      <c r="C24" s="125"/>
+      <c r="D24" s="135" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="59">
+      <c r="E24" s="127">
         <v>-2.58E-2</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="111">
         <f>MATCH($D24,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>22</v>
       </c>
-      <c r="G24" s="37">
+      <c r="G24" s="134">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F24,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="37">
+      <c r="H24" s="134">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F24,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I24" s="33" t="str">
+      <c r="I24" s="128" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34" t="str">
+      <c r="J24" s="129"/>
+      <c r="K24" s="129" t="str">
         <f t="shared" si="3"/>
         <v>YEARS_SINCE_TNC_RAIL2_MIDLOW_FAC</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="111">
         <f>MATCH($K24,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>36</v>
       </c>
-      <c r="M24" s="32">
+      <c r="M24" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="N24" s="32">
+      <c r="N24" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="O24" s="32">
+      <c r="O24" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="P24" s="32">
+      <c r="P24" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Q24" s="32">
+      <c r="Q24" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="R24" s="32">
+      <c r="R24" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="S24" s="32">
+      <c r="S24" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="T24" s="32">
+      <c r="T24" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="U24" s="32">
+      <c r="U24" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="V24" s="32">
+      <c r="V24" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="W24" s="32">
+      <c r="W24" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="X24" s="32">
+      <c r="X24" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Y24" s="32">
+      <c r="Y24" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Z24" s="32">
+      <c r="Z24" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AA24" s="32">
+      <c r="AA24" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AB24" s="32">
+      <c r="AB24" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L24,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AC24" s="35">
+      <c r="AC24" s="130">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD24" s="36">
+      <c r="AD24" s="131">
         <f>AC24/G29</f>
         <v>0</v>
       </c>
@@ -5430,113 +5564,113 @@
     </row>
     <row r="25" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="124" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="9" t="s">
+      <c r="C25" s="125"/>
+      <c r="D25" s="111" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="59">
+      <c r="E25" s="127">
         <v>1.46E-2</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="111">
         <f>MATCH($D25,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>23</v>
       </c>
-      <c r="G25" s="37">
+      <c r="G25" s="134">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F25,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="37">
+      <c r="H25" s="134">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F25,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="I25" s="33" t="str">
+      <c r="I25" s="128" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="J25" s="34" t="str">
+      <c r="J25" s="129" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K25" s="34" t="str">
+      <c r="K25" s="129" t="str">
         <f t="shared" si="3"/>
         <v>BIKE_SHARE_FAC</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="111">
         <f>MATCH($K25,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>37</v>
       </c>
-      <c r="M25" s="32">
+      <c r="M25" s="126">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="N25" s="32">
+      <c r="N25" s="126">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="O25" s="32">
+      <c r="O25" s="126">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="P25" s="32">
+      <c r="P25" s="126">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Q25" s="32">
+      <c r="Q25" s="126">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="R25" s="32">
+      <c r="R25" s="126">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>2734634.3054004</v>
       </c>
-      <c r="S25" s="32">
+      <c r="S25" s="126">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="T25" s="32">
+      <c r="T25" s="126">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>2278562.3532980499</v>
       </c>
-      <c r="U25" s="32">
+      <c r="U25" s="126">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>1698305.52754262</v>
       </c>
-      <c r="V25" s="32">
+      <c r="V25" s="126">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>989105.41772997798</v>
       </c>
-      <c r="W25" s="32">
+      <c r="W25" s="126">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="X25" s="32">
+      <c r="X25" s="126">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>10676855.2261317</v>
       </c>
-      <c r="Y25" s="32">
+      <c r="Y25" s="126">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>9214414.4661997408</v>
       </c>
-      <c r="Z25" s="32">
+      <c r="Z25" s="126">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>2197032.9831991899</v>
       </c>
-      <c r="AA25" s="32">
+      <c r="AA25" s="126">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AB25" s="32">
+      <c r="AB25" s="126">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L25,FALSE))</f>
         <v>425279.174070312</v>
       </c>
-      <c r="AC25" s="35">
+      <c r="AC25" s="130">
         <f t="shared" si="4"/>
         <v>30214189.453571994</v>
       </c>
-      <c r="AD25" s="36">
+      <c r="AD25" s="131">
         <f>AC25/G29</f>
         <v>1.524424878835307E-2</v>
       </c>
@@ -5544,113 +5678,113 @@
     </row>
     <row r="26" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="136" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="10" t="s">
+      <c r="C26" s="137"/>
+      <c r="D26" s="138" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="60">
+      <c r="E26" s="139">
         <v>-4.8399999999999999E-2</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="138">
         <f>MATCH($D26,FAC_TOTALS_APTA!$A$2:$BS$2,)</f>
         <v>24</v>
       </c>
-      <c r="G26" s="39">
+      <c r="G26" s="140">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F26,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="39">
+      <c r="H26" s="140">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BS$143,$F26,FALSE)</f>
         <v>0.66313958588773203</v>
       </c>
-      <c r="I26" s="40" t="str">
+      <c r="I26" s="141" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="J26" s="41" t="str">
+      <c r="J26" s="142" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K26" s="41" t="str">
+      <c r="K26" s="142" t="str">
         <f t="shared" si="3"/>
         <v>scooter_flag_FAC</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26" s="138">
         <f>MATCH($K26,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>38</v>
       </c>
-      <c r="M26" s="42">
+      <c r="M26" s="143">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="N26" s="42">
+      <c r="N26" s="143">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="O26" s="42">
+      <c r="O26" s="143">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="P26" s="42">
+      <c r="P26" s="143">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Q26" s="42">
+      <c r="Q26" s="143">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="R26" s="42">
+      <c r="R26" s="143">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="S26" s="42">
+      <c r="S26" s="143">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="T26" s="42">
+      <c r="T26" s="143">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="U26" s="42">
+      <c r="U26" s="143">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="V26" s="42">
+      <c r="V26" s="143">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="W26" s="42">
+      <c r="W26" s="143">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="X26" s="42">
+      <c r="X26" s="143">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Y26" s="42">
+      <c r="Y26" s="143">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Z26" s="42">
+      <c r="Z26" s="143">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AA26" s="42">
+      <c r="AA26" s="143">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AB26" s="42">
+      <c r="AB26" s="143">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L26,FALSE))</f>
         <v>-61224588.800484002</v>
       </c>
-      <c r="AC26" s="43">
+      <c r="AC26" s="144">
         <f t="shared" si="4"/>
         <v>-61224588.800484002</v>
       </c>
-      <c r="AD26" s="44">
+      <c r="AD26" s="145">
         <f>AC26/G29</f>
         <v>-3.089021683250396E-2</v>
       </c>
@@ -5658,96 +5792,96 @@
     </row>
     <row r="27" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="146" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="45" t="s">
+      <c r="C27" s="147"/>
+      <c r="D27" s="146" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="47"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51" t="str">
+      <c r="E27" s="148"/>
+      <c r="F27" s="149"/>
+      <c r="G27" s="150"/>
+      <c r="H27" s="150"/>
+      <c r="I27" s="151"/>
+      <c r="J27" s="152"/>
+      <c r="K27" s="152" t="str">
         <f t="shared" si="3"/>
         <v>New_Reporter_FAC</v>
       </c>
-      <c r="L27" s="48">
+      <c r="L27" s="149">
         <f>MATCH($K27,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>42</v>
       </c>
-      <c r="M27" s="49">
+      <c r="M27" s="150">
         <f>IF(M11=0,0,VLOOKUP(M11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="N27" s="49">
+      <c r="N27" s="150">
         <f>IF(N11=0,0,VLOOKUP(N11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="O27" s="49">
+      <c r="O27" s="150">
         <f>IF(O11=0,0,VLOOKUP(O11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="P27" s="49">
+      <c r="P27" s="150">
         <f>IF(P11=0,0,VLOOKUP(P11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Q27" s="49">
+      <c r="Q27" s="150">
         <f>IF(Q11=0,0,VLOOKUP(Q11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="R27" s="49">
+      <c r="R27" s="150">
         <f>IF(R11=0,0,VLOOKUP(R11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="S27" s="49">
+      <c r="S27" s="150">
         <f>IF(S11=0,0,VLOOKUP(S11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="T27" s="49">
+      <c r="T27" s="150">
         <f>IF(T11=0,0,VLOOKUP(T11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="U27" s="49">
+      <c r="U27" s="150">
         <f>IF(U11=0,0,VLOOKUP(U11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="V27" s="49">
+      <c r="V27" s="150">
         <f>IF(V11=0,0,VLOOKUP(V11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="W27" s="49">
+      <c r="W27" s="150">
         <f>IF(W11=0,0,VLOOKUP(W11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="X27" s="49">
+      <c r="X27" s="150">
         <f>IF(X11=0,0,VLOOKUP(X11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Y27" s="49">
+      <c r="Y27" s="150">
         <f>IF(Y11=0,0,VLOOKUP(Y11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="Z27" s="49">
+      <c r="Z27" s="150">
         <f>IF(Z11=0,0,VLOOKUP(Z11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AA27" s="49">
+      <c r="AA27" s="150">
         <f>IF(AA11=0,0,VLOOKUP(AA11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AB27" s="49">
+      <c r="AB27" s="150">
         <f>IF(AB11=0,0,VLOOKUP(AB11,FAC_TOTALS_APTA!$A$4:$BS$143,$L27,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AC27" s="52">
+      <c r="AC27" s="153">
         <f>SUM(M27:AB27)</f>
         <v>0</v>
       </c>
-      <c r="AD27" s="53">
+      <c r="AD27" s="154">
         <f>AC27/G29</f>
         <v>0</v>
       </c>
@@ -5755,192 +5889,192 @@
     </row>
     <row r="28" spans="1:31" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="111"/>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="124" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="9" t="s">
+      <c r="C28" s="125"/>
+      <c r="D28" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="59"/>
-      <c r="F28" s="9">
+      <c r="E28" s="127"/>
+      <c r="F28" s="111">
         <f>MATCH($D28,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>9</v>
       </c>
-      <c r="G28" s="117">
+      <c r="G28" s="126">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BS$143,$F28,FALSE)</f>
         <v>1878108677.18068</v>
       </c>
-      <c r="H28" s="117">
+      <c r="H28" s="126">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BQ$143,$F28,FALSE)</f>
         <v>1858989004.65239</v>
       </c>
-      <c r="I28" s="119">
+      <c r="I28" s="155">
         <f t="shared" ref="I28:I29" si="5">H28/G28-1</f>
         <v>-1.0180280172599754E-2</v>
       </c>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="32">
+      <c r="J28" s="129"/>
+      <c r="K28" s="129"/>
+      <c r="L28" s="111"/>
+      <c r="M28" s="126">
         <f t="shared" ref="M28:AB28" si="6">SUM(M13:M18)</f>
         <v>133756657.0200754</v>
       </c>
-      <c r="N28" s="32">
+      <c r="N28" s="126">
         <f t="shared" si="6"/>
         <v>46470142.518143296</v>
       </c>
-      <c r="O28" s="32">
+      <c r="O28" s="126">
         <f t="shared" si="6"/>
         <v>17744997.661508691</v>
       </c>
-      <c r="P28" s="32">
+      <c r="P28" s="126">
         <f t="shared" si="6"/>
         <v>66913006.814874768</v>
       </c>
-      <c r="Q28" s="32">
+      <c r="Q28" s="126">
         <f t="shared" si="6"/>
         <v>25829062.829311315</v>
       </c>
-      <c r="R28" s="32">
+      <c r="R28" s="126">
         <f t="shared" si="6"/>
         <v>90406200.196528465</v>
       </c>
-      <c r="S28" s="32">
+      <c r="S28" s="126">
         <f t="shared" si="6"/>
         <v>-142094812.28520772</v>
       </c>
-      <c r="T28" s="32">
+      <c r="T28" s="126">
         <f t="shared" si="6"/>
         <v>-35813865.421329997</v>
       </c>
-      <c r="U28" s="32">
+      <c r="U28" s="126">
         <f t="shared" si="6"/>
-        <v>40610269.852067843</v>
-      </c>
-      <c r="V28" s="32">
+        <v>80253541.276620731</v>
+      </c>
+      <c r="V28" s="126">
         <f t="shared" si="6"/>
         <v>-20593785.247955505</v>
       </c>
-      <c r="W28" s="32">
+      <c r="W28" s="126">
         <f t="shared" si="6"/>
         <v>6766526.0894256001</v>
       </c>
-      <c r="X28" s="32">
+      <c r="X28" s="126">
         <f t="shared" si="6"/>
         <v>-2311046.8144458691</v>
       </c>
-      <c r="Y28" s="32">
+      <c r="Y28" s="126">
         <f t="shared" si="6"/>
         <v>-65027528.0699476</v>
       </c>
-      <c r="Z28" s="32">
+      <c r="Z28" s="126">
         <f t="shared" si="6"/>
         <v>-22642722.769414511</v>
       </c>
-      <c r="AA28" s="32">
+      <c r="AA28" s="126">
         <f t="shared" si="6"/>
         <v>57562177.306293428</v>
       </c>
-      <c r="AB28" s="32">
+      <c r="AB28" s="126">
         <f t="shared" si="6"/>
         <v>48172701.040468849</v>
       </c>
-      <c r="AC28" s="35">
+      <c r="AC28" s="130">
         <f>H28-G28</f>
         <v>-19119672.528290033</v>
       </c>
-      <c r="AD28" s="36">
+      <c r="AD28" s="131">
         <f>I28</f>
         <v>-1.0180280172599754E-2</v>
       </c>
       <c r="AE28" s="111"/>
     </row>
     <row r="29" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="156" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26" t="s">
+      <c r="C29" s="157"/>
+      <c r="D29" s="157" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26">
+      <c r="E29" s="157"/>
+      <c r="F29" s="157">
         <f>MATCH($D29,FAC_TOTALS_APTA!$A$2:$BQ$2,)</f>
         <v>7</v>
       </c>
-      <c r="G29" s="118">
+      <c r="G29" s="123">
         <f>VLOOKUP(G11,FAC_TOTALS_APTA!$A$4:$BQ$143,$F29,FALSE)</f>
         <v>1982005795.96</v>
       </c>
-      <c r="H29" s="118">
+      <c r="H29" s="123">
         <f>VLOOKUP(H11,FAC_TOTALS_APTA!$A$4:$BQ$143,$F29,FALSE)</f>
         <v>1830572626.3499899</v>
       </c>
-      <c r="I29" s="120">
+      <c r="I29" s="158">
         <f t="shared" si="5"/>
         <v>-7.6403999382182564E-2</v>
       </c>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="26"/>
-      <c r="U29" s="26"/>
-      <c r="V29" s="26"/>
-      <c r="W29" s="26"/>
-      <c r="X29" s="26"/>
-      <c r="Y29" s="26"/>
-      <c r="Z29" s="26"/>
-      <c r="AA29" s="26"/>
-      <c r="AB29" s="26"/>
-      <c r="AC29" s="55">
+      <c r="J29" s="159"/>
+      <c r="K29" s="159"/>
+      <c r="L29" s="157"/>
+      <c r="M29" s="157"/>
+      <c r="N29" s="157"/>
+      <c r="O29" s="157"/>
+      <c r="P29" s="157"/>
+      <c r="Q29" s="157"/>
+      <c r="R29" s="157"/>
+      <c r="S29" s="157"/>
+      <c r="T29" s="157"/>
+      <c r="U29" s="157"/>
+      <c r="V29" s="157"/>
+      <c r="W29" s="157"/>
+      <c r="X29" s="157"/>
+      <c r="Y29" s="157"/>
+      <c r="Z29" s="157"/>
+      <c r="AA29" s="157"/>
+      <c r="AB29" s="157"/>
+      <c r="AC29" s="160">
         <f>H29-G29</f>
         <v>-151433169.61001015</v>
       </c>
-      <c r="AD29" s="56">
+      <c r="AD29" s="161">
         <f>I29</f>
         <v>-7.6403999382182564E-2</v>
       </c>
     </row>
     <row r="30" spans="1:31" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="61" t="s">
+      <c r="B30" s="162" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="62"/>
-      <c r="K30" s="62"/>
-      <c r="L30" s="62"/>
-      <c r="M30" s="62"/>
-      <c r="N30" s="62"/>
-      <c r="O30" s="62"/>
-      <c r="P30" s="62"/>
-      <c r="Q30" s="62"/>
-      <c r="R30" s="62"/>
-      <c r="S30" s="62"/>
-      <c r="T30" s="62"/>
-      <c r="U30" s="62"/>
-      <c r="V30" s="62"/>
-      <c r="W30" s="62"/>
-      <c r="X30" s="62"/>
-      <c r="Y30" s="62"/>
-      <c r="Z30" s="62"/>
-      <c r="AA30" s="62"/>
-      <c r="AB30" s="62"/>
-      <c r="AC30" s="62"/>
-      <c r="AD30" s="56">
+      <c r="C30" s="163"/>
+      <c r="D30" s="163"/>
+      <c r="E30" s="164"/>
+      <c r="F30" s="163"/>
+      <c r="G30" s="163"/>
+      <c r="H30" s="163"/>
+      <c r="I30" s="165"/>
+      <c r="J30" s="163"/>
+      <c r="K30" s="163"/>
+      <c r="L30" s="163"/>
+      <c r="M30" s="163"/>
+      <c r="N30" s="163"/>
+      <c r="O30" s="163"/>
+      <c r="P30" s="163"/>
+      <c r="Q30" s="163"/>
+      <c r="R30" s="163"/>
+      <c r="S30" s="163"/>
+      <c r="T30" s="163"/>
+      <c r="U30" s="163"/>
+      <c r="V30" s="163"/>
+      <c r="W30" s="163"/>
+      <c r="X30" s="163"/>
+      <c r="Y30" s="163"/>
+      <c r="Z30" s="163"/>
+      <c r="AA30" s="163"/>
+      <c r="AB30" s="163"/>
+      <c r="AC30" s="163"/>
+      <c r="AD30" s="161">
         <f>AD29-AD28</f>
         <v>-6.622371920958281E-2</v>
       </c>
@@ -12793,6 +12927,7 @@
     <sheetView showGridLines="0" topLeftCell="A89" workbookViewId="0">
       <selection activeCell="B114" sqref="B114:AD117"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21965,6 +22100,7 @@
     <sheetView showGridLines="0" topLeftCell="A77" workbookViewId="0">
       <selection activeCell="B115" sqref="B115:AD118"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31189,9 +31325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AG119"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="AF28" sqref="AF28"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -40399,11 +40534,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BU143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="1">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -40413,20 +40548,26 @@
     <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
     <col min="6" max="7" width="16.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.125" style="2" customWidth="1"/>
     <col min="10" max="10" width="15.375" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.375" style="4" customWidth="1"/>
-    <col min="18" max="26" width="14.625" style="4" customWidth="1"/>
-    <col min="27" max="27" width="18.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="11.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22" style="2" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="27" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.625" style="2" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="22.875" bestFit="1" customWidth="1"/>
@@ -42157,10 +42298,12 @@
         <v>56740870.446837001</v>
       </c>
       <c r="AC13">
-        <v>8606390.5169233494</v>
+        <f>SUM(M13:AB13)</f>
+        <v>48249661.941476241</v>
       </c>
       <c r="AD13">
-        <v>3860938.6203019</v>
+        <f>AC13/G29</f>
+        <v>5.3162988831291169E-2</v>
       </c>
       <c r="AE13">
         <v>-8375600.4785643797</v>

</xml_diff>